<commit_message>
update all script and file in folder
</commit_message>
<xml_diff>
--- a/OnBoard/data/StationTablet_TEMPLATE.xlsx
+++ b/OnBoard/data/StationTablet_TEMPLATE.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.luzi\OneDrive - CNR\CNR\SoleMon\Github\SoleMon_project\OnBoard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.luzi\OneDrive - CNR\CNR\SoleMon\Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Station" sheetId="1" r:id="rId1"/>
     <sheet name="NotesCala" sheetId="2" r:id="rId2"/>
     <sheet name="Samples onboard" sheetId="3" r:id="rId3"/>
     <sheet name="Species" sheetId="5" r:id="rId4"/>
-    <sheet name="Notes for compilation" sheetId="4" r:id="rId5"/>
+    <sheet name="Note di compilazione" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Species!$D$1:$E$1274</definedName>
@@ -8045,8 +8045,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CasellaDiTesto 1">
@@ -9753,7 +9753,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CasellaDiTesto 1">

</xml_diff>